<commit_message>
19a, 20a, battle flags, ballistae
</commit_message>
<xml_diff>
--- a/Chapter progress.xlsx
+++ b/Chapter progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FE6inFE8\FE6-in-FE8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F92B52-2806-4CBC-9983-8135F1CF2FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F148867E-B7AF-4528-9796-0BF24B18C5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28320" yWindow="7860" windowWidth="21885" windowHeight="12090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -777,7 +777,7 @@
       <c r="B28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="4"/>
+      <c r="C28" s="3"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -786,7 +786,7 @@
       <c r="B29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="4"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>

</xml_diff>

<commit_message>
YOU'RE GOING TO SACAE
</commit_message>
<xml_diff>
--- a/Chapter progress.xlsx
+++ b/Chapter progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FE6inFE8\FE6-in-FE8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F148867E-B7AF-4528-9796-0BF24B18C5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E781A4E0-B8C0-4F34-98FB-0FE1CD408D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28320" yWindow="7860" windowWidth="21885" windowHeight="12090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Number</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Room and bottom-half reinforcements not implemented</t>
+  </si>
+  <si>
+    <t>Tents ambush not implemented, unclear how it works in fe6 (wiki wrong?)</t>
   </si>
 </sst>
 </file>
@@ -491,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,7 +505,7 @@
     <col min="4" max="4" width="13.21875" customWidth="1"/>
     <col min="5" max="5" width="19.77734375" customWidth="1"/>
     <col min="6" max="6" width="12.77734375" customWidth="1"/>
-    <col min="7" max="7" width="61.6640625" customWidth="1"/>
+    <col min="7" max="7" width="63.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
@@ -795,7 +798,7 @@
       <c r="B30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="4"/>
+      <c r="C30" s="3"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -804,7 +807,7 @@
       <c r="B31" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="4"/>
+      <c r="C31" s="3"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -813,16 +816,19 @@
       <c r="B32" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="4"/>
+      <c r="C32" s="3"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
+      <c r="G32" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="4"/>
+      <c r="C33" s="3"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>

</xml_diff>

<commit_message>
fix + escape points
</commit_message>
<xml_diff>
--- a/Chapter progress.xlsx
+++ b/Chapter progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FE6inFE8\FE6-in-FE8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460BCF57-A13C-4B85-8DA1-5099CFE761F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFBDD81-9162-4D89-92D3-8B7DA0C45373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4164" yWindow="2520" windowWidth="25824" windowHeight="12096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-456" yWindow="5196" windowWidth="25824" windowHeight="12096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Number</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Chest and the other traps not implemented, seems like it's gonna be tricky with them</t>
+  </si>
+  <si>
+    <t>Epilogue, leg weapons check not implemented</t>
   </si>
 </sst>
 </file>
@@ -491,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -867,16 +870,19 @@
       <c r="B38" s="1">
         <v>22</v>
       </c>
-      <c r="C38" s="4"/>
+      <c r="C38" s="3"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
+      <c r="G38" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B39" s="1">
         <v>23</v>
       </c>
-      <c r="C39" s="4"/>
+      <c r="C39" s="3"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>

</xml_diff>

<commit_message>
fog, clarine talk ai, todos
</commit_message>
<xml_diff>
--- a/Chapter progress.xlsx
+++ b/Chapter progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FE6inFE8\FE6-in-FE8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1093BD-B6B1-4035-8503-8228C41B4586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F48E7D-160A-48D1-86E4-427471A89282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20880" yWindow="7845" windowWidth="16785" windowHeight="12090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Number</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Extra notes</t>
   </si>
   <si>
-    <t>Clarine needs "Talk to Roy AI"</t>
-  </si>
-  <si>
     <t>Completable?</t>
   </si>
   <si>
@@ -115,9 +112,6 @@
   </si>
   <si>
     <t>Fadeins etc</t>
-  </si>
-  <si>
-    <t>Tents ambush not implemented, unclear how it works in fe6 (wiki wrong?)</t>
   </si>
   <si>
     <t>Chest and the other traps not implemented, seems like it's gonna be tricky with them</t>
@@ -485,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,13 +495,13 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
@@ -515,16 +509,16 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
         <v>21</v>
@@ -565,9 +559,6 @@
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
@@ -731,7 +722,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
@@ -796,9 +787,6 @@
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="G32" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
@@ -845,7 +833,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
@@ -857,7 +845,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
replace bard refresh, ch fixes
</commit_message>
<xml_diff>
--- a/Chapter progress.xlsx
+++ b/Chapter progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FE6inFE8\FE6-in-FE8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AA2CA1-A6E2-46CC-B7A1-D705BA6D93A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0886655-415D-49F1-82A4-E688FEDCDEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18780" yWindow="6090" windowWidth="18645" windowHeight="10455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22875" yWindow="8340" windowWidth="18645" windowHeight="10455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -479,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,8 +619,8 @@
         <v>2</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
@@ -628,8 +628,8 @@
         <v>3</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
@@ -637,8 +637,8 @@
         <v>4</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
@@ -646,8 +646,8 @@
         <v>5</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
@@ -655,8 +655,8 @@
         <v>12</v>
       </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
@@ -664,8 +664,8 @@
         <v>6</v>
       </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">

</xml_diff>